<commit_message>
Removed cancelled item in overall report
</commit_message>
<xml_diff>
--- a/Damage Summary Report.xlsx
+++ b/Damage Summary Report.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
-  <si>
-    <t>Damage Summary Report November2020</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
+  <si>
+    <t>Damage Summary Report November2017</t>
   </si>
   <si>
     <t>No.</t>
@@ -41,6 +41,18 @@
     <t>Item Description</t>
   </si>
   <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Serial No.</t>
+  </si>
+  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -69,6 +81,291 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>2020-06-17</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2020-06-1001</t>
+  </si>
+  <si>
+    <t>Furniture, Fixtures and Equipment</t>
+  </si>
+  <si>
+    <t>Marianita Tabilla</t>
+  </si>
+  <si>
+    <t>HDD 500GB</t>
+  </si>
+  <si>
+    <t>Western Digital</t>
+  </si>
+  <si>
+    <t>WD5000AADS-57S9B1</t>
+  </si>
+  <si>
+    <t>WCAV9M637403</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00 </t>
+  </si>
+  <si>
+    <t>Jason Flor</t>
+  </si>
+  <si>
+    <t>-Slow processing of App Files( It takes minutes to process)
+-Suddenly the screen turned blue (BSOD)</t>
+  </si>
+  <si>
+    <t>-HDD Health 12%
+-Tried several repair and reformat of operating system but the  performance is running low</t>
+  </si>
+  <si>
+    <t>-Use temporary spare HDD
+-Purchase new HDD</t>
+  </si>
+  <si>
+    <t>2020-07-02</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2020-07-1001</t>
+  </si>
+  <si>
+    <t>All Trading Personnel</t>
+  </si>
+  <si>
+    <t>LED TV 40'</t>
+  </si>
+  <si>
+    <t>TCL</t>
+  </si>
+  <si>
+    <t>IT20190315</t>
+  </si>
+  <si>
+    <t>Caesariane Jo</t>
+  </si>
+  <si>
+    <t>Black out screen</t>
+  </si>
+  <si>
+    <t>if you turn off the TV, after a few minutes it automatically turn off/ blackout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2020-07-06</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2020-07-1002</t>
+  </si>
+  <si>
+    <t>IT20190364</t>
+  </si>
+  <si>
+    <t>Joemar De Los Santos</t>
+  </si>
+  <si>
+    <t>if you turn of the TV, after a few minutes it automatically turn off/ blackout</t>
+  </si>
+  <si>
+    <t>for check up/ repair</t>
+  </si>
+  <si>
+    <t>2020-07-22</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2020-07-1003</t>
+  </si>
+  <si>
+    <t>External Hard Drive 1TB</t>
+  </si>
+  <si>
+    <t>SEAGATE</t>
+  </si>
+  <si>
+    <t>SRD00F1</t>
+  </si>
+  <si>
+    <t>NA9VR3ZD</t>
+  </si>
+  <si>
+    <t>Lost July 13, 2020 when we process the back up files to the external drive it does not function</t>
+  </si>
+  <si>
+    <t>The hard drive cannot open? Ticking or clicking sound (Scratching)</t>
+  </si>
+  <si>
+    <t>Unrepairable/Physical damage on internal platter</t>
+  </si>
+  <si>
+    <t>2020-09-24</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2020-09-1001</t>
+  </si>
+  <si>
+    <t>Jonah Faye Benares</t>
+  </si>
+  <si>
+    <t>Laptop 14inches, Intel Core i5-5200U CPU @ 2.20GHz, 4GB RAM, 1TB HDD</t>
+  </si>
+  <si>
+    <t>Acer</t>
+  </si>
+  <si>
+    <t>NXV9USP018602033587600</t>
+  </si>
+  <si>
+    <t>I arrived at the office and immediately turned on my laptop. When I use the mouse and keyboard to check it, it doesn't respond well and some parts are blinking. I had Jushkyle checked it, he restarted twice and it was fine. But after a while it came back again. Already tried two different mouse and track pad, also disabled the 3rd party keyboard and used its built in keyboard but it's still the same. Also tried formatting it but wasn't done because I cannot control it anymore.</t>
+  </si>
+  <si>
+    <t>Not responding well.</t>
+  </si>
+  <si>
+    <t>To be repaired to check the source of the damage (software of hardware).</t>
+  </si>
+  <si>
+    <t>2020-11-24</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2020-11-1001</t>
+  </si>
+  <si>
+    <t>Alma Bella  Gabitoya</t>
+  </si>
+  <si>
+    <t>VGA</t>
+  </si>
+  <si>
+    <t>IT20190295</t>
+  </si>
+  <si>
+    <t>Alma Bella Redocto Gabitoya</t>
+  </si>
+  <si>
+    <t>The VGA is not functioning well.</t>
+  </si>
+  <si>
+    <t>The Monitor is not clear</t>
+  </si>
+  <si>
+    <t>Change the VGA</t>
+  </si>
+  <si>
+    <t>2021-01-26</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2021-01-1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babylyn Providencia
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printer Cord </t>
+  </si>
+  <si>
+    <t>IT20190388</t>
+  </si>
+  <si>
+    <t>2019-10-08</t>
+  </si>
+  <si>
+    <t>Babylyn Providencia</t>
+  </si>
+  <si>
+    <t>unable to print</t>
+  </si>
+  <si>
+    <t>-The pc/laptop cant detect the cord.
+-Tried the cord to different printer and still cant detect it.</t>
+  </si>
+  <si>
+    <t>Replace item</t>
+  </si>
+  <si>
+    <t>2021-02-18</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2021-02-1001</t>
+  </si>
+  <si>
+    <t>Syndey Sinoro</t>
+  </si>
+  <si>
+    <t>UPS 650VA</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>Back UPS 650</t>
+  </si>
+  <si>
+    <t>9B1646A05761</t>
+  </si>
+  <si>
+    <t>malfunction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ups have constant beeping generally means the ups is very low on battery power and battery did not charge anymore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">replace new battery </t>
+  </si>
+  <si>
+    <t>2021-03-10</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2021-03-1001</t>
+  </si>
+  <si>
+    <t>Ruth Jan Destacamento</t>
+  </si>
+  <si>
+    <t>UPS 720VA</t>
+  </si>
+  <si>
+    <t>ILogic</t>
+  </si>
+  <si>
+    <t>Blazer 720VA</t>
+  </si>
+  <si>
+    <t>All the equipment of Ms. Ruth shutdown in times of brownout.</t>
+  </si>
+  <si>
+    <t>The UPS is not charging.</t>
+  </si>
+  <si>
+    <t>Replace Battery</t>
+  </si>
+  <si>
+    <t>2021-03-12</t>
+  </si>
+  <si>
+    <t>CENPRI-B-2021-03-1002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zyndyryn </t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>IT20190250</t>
+  </si>
+  <si>
+    <t>All the equipment of Ms. Zyndyryn shutdown in times of brownout. 
+Ms. Zyndyryn and Ms. Marian shares UPS which makes the battery to drain.</t>
+  </si>
+  <si>
+    <t>Replace battery</t>
   </si>
 </sst>
 </file>
@@ -136,9 +433,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -445,7 +751,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -455,83 +761,655 @@
   <cols>
     <col min="1" max="1" width="44.703369" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="14.996338" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11.282959" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="8.426514" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="8.426514" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="39.990234" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="37.8479" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="3.570557" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="3.570557" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="13.139648" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="12.139893" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="26.422119" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="27.421875" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="14.139404" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="7.426758" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="81.265869" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="26.993408" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="3.570557" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="15.996094" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="15.996094" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="13.139648" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="568.575439" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="135.53833" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="85.979004" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="7.426758" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:21">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="R2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1">
+        <v>231701504407</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="U12" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>